<commit_message>
Base Page of BAJAJ-PL Analysis
</commit_message>
<xml_diff>
--- a/media/BAJAJ-CD/MIS/BAJAJ TC-WISE MIS.xlsx
+++ b/media/BAJAJ-CD/MIS/BAJAJ TC-WISE MIS.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -534,11 +534,7 @@
           <t>O290</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>O254</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>LOWER MANAGEMENT</t>
@@ -556,17 +552,17 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>BAJAJ</t>
+          <t>IDFC</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>TW</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -599,11 +595,7 @@
           <t>O194</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>O281</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
           <t>LOWER MANAGEMENT</t>
@@ -729,11 +721,7 @@
           <t>O269</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>O254</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>LOWER MANAGEMENT</t>
@@ -751,7 +739,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">

</xml_diff>